<commit_message>
updated github hyperlink and congressional insights
</commit_message>
<xml_diff>
--- a/data/potential_usdot_emphasis_area_data.xlsx
+++ b/data/potential_usdot_emphasis_area_data.xlsx
@@ -45,7 +45,7 @@
     <t>Share of the population under 18 are fromUS Census Bureau American Community Survey 5-yr data, Detailed Table B01001. The 5-year data vintgae is used to allow downlaoding the data for all cities and towns as 1 year data is only available for geographies with more than 65,000 people in them.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">geography</t>
@@ -4075,7 +4075,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>45717</v>
+        <v>45720</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1"/>

</xml_diff>